<commit_message>
new population plotting code
</commit_message>
<xml_diff>
--- a/src/code/templates/NonmemFieldDicitonary.xlsx
+++ b/src/code/templates/NonmemFieldDicitonary.xlsx
@@ -173,9 +173,6 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>Organism|Gender</t>
-  </si>
-  <si>
     <t>units are defined in corresponding output definitions</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   <si>
     <t>name of column in nonmem file; 
 columns with beginning# can not be evaluated</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -769,10 +769,10 @@
         <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Meanmodel workflow and new testcases (#6)
* new population plotting code

* add mean model workflow.m
automatic workflow.m creation
update on tests

* new if nInd > 1000 save simulation results in bunches
parallelisation (use same structurs and functions) of Individual simulation and Population simulation
</commit_message>
<xml_diff>
--- a/src/code/templates/NonmemFieldDicitonary.xlsx
+++ b/src/code/templates/NonmemFieldDicitonary.xlsx
@@ -173,9 +173,6 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>Organism|Gender</t>
-  </si>
-  <si>
     <t>units are defined in corresponding output definitions</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   <si>
     <t>name of column in nonmem file; 
 columns with beginning# can not be evaluated</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -769,10 +769,10 @@
         <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">

</xml_diff>